<commit_message>
Updated README and demo
</commit_message>
<xml_diff>
--- a/demo/template.xlsx
+++ b/demo/template.xlsx
@@ -1,21 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivahaev/Documents/golang/src/candy/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B841B51-B2FB-4CFC-A7D8-563506787ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,31 +33,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Hello {{name}}</t>
   </si>
   <si>
+    <t>Here is a list of your items</t>
+  </si>
+  <si>
+    <t>{{groupHeader}}</t>
+  </si>
+  <si>
     <t>{{nameHeader}}</t>
   </si>
   <si>
     <t>{{quantityHeader}}</t>
   </si>
   <si>
-    <t>Here is a list of your items</t>
+    <t>{{range groups}}</t>
+  </si>
+  <si>
+    <t>{{if important}}</t>
+  </si>
+  <si>
+    <t>{{name}}</t>
+  </si>
+  <si>
+    <t>{{else}}</t>
+  </si>
+  <si>
+    <t>{{end}}</t>
   </si>
   <si>
     <t>{{items.name}}</t>
   </si>
   <si>
     <t>{{items.quantity}}</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>{{total}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,8 +104,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,8 +125,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -95,15 +147,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -111,29 +165,42 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -141,33 +208,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -435,56 +532,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.625" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" ht="21">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75">
+      <c r="A5" s="2"/>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="s">
+    <row r="6" spans="1:5" ht="15.75">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75">
+      <c r="B8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75">
+      <c r="B10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75">
+      <c r="B13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="19" ht="15.75"/>
+    <row r="20" ht="15.75"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A4:E4"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>